<commit_message>
Se agregó hoja de mitigación de riesgos
</commit_message>
<xml_diff>
--- a/tabla-riesgos .xlsx
+++ b/tabla-riesgos .xlsx
@@ -1,25 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xavie\Documents\Proyecto_Final\PoryectoFinalSIDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DEFE4F-0A4F-416F-A516-AFCCFB1E79A1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="164">
   <si>
     <t>Codigo del riesgo</t>
   </si>
@@ -379,12 +388,144 @@
   </si>
   <si>
     <t>Rechazo del producto por parte del usuario (no cumple los criterios de aceptación)</t>
+  </si>
+  <si>
+    <t>Nivel del riesgo</t>
+  </si>
+  <si>
+    <t>Plan de Mitigación</t>
+  </si>
+  <si>
+    <t>Se debe contar con un analista con experiencia para que realice el levantamineto de riesgos de manera optima</t>
+  </si>
+  <si>
+    <t>Plan de Contingencia</t>
+  </si>
+  <si>
+    <t>Se debe organizar reuniones con el cliente y especificar requerimeintos faltantes</t>
+  </si>
+  <si>
+    <t>Revisar documentación de versiones y de plugins o depencias que se usarán.</t>
+  </si>
+  <si>
+    <t>Buscar herramientas alternativas que sean compatibles con los medios utilizados.</t>
+  </si>
+  <si>
+    <t>Evitar contratación de desarrolladores inexpertos Ofrecer capacitaciones al equipo de desarrollo y plantear tiempos de holgura para el aprendizaje</t>
+  </si>
+  <si>
+    <t>Abrir convocatoria para capacitación en horarios adicionales</t>
+  </si>
+  <si>
+    <t>Trabajar con una versión estable o conocidad</t>
+  </si>
+  <si>
+    <t>Solicitar documentación de alguien experto o dedicar tiempo recursos para aprender las nuevas carácterísticas</t>
+  </si>
+  <si>
+    <t>Contratar más gente experta o siempre estimar 20% mas de recurso</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Modificar linea base de desarrollo y segmentar por modulos</t>
+  </si>
+  <si>
+    <t>Reuniones períodicas con el Usuario, también por fases</t>
+  </si>
+  <si>
+    <t>Reuniones con el cliente para identificar que no le gusto y concretar entrega</t>
+  </si>
+  <si>
+    <t>Listar proveedores que cumplan con los requisitos. Usar otro proveedor que use  las mismas tecnologias.Ver clausulas de contrato</t>
+  </si>
+  <si>
+    <t>Solicitar cumplimiento de clausulas de contrato. Revisar tiempos de entrega.Renegociar con el cliente.</t>
+  </si>
+  <si>
+    <t>Conocer muy bien el Manejador de transacciones.Pruebas constantes de concepto.Definir reglas y control de errores.</t>
+  </si>
+  <si>
+    <t>Acudir a los resultados en primera medida. Ajustar Modelo.</t>
+  </si>
+  <si>
+    <t>Buscar soporte del proveedor.Cambio de proveedor de servicios de comunicaciones.</t>
+  </si>
+  <si>
+    <t>Que una persona experta plantee o analice las póliticas de calidad .</t>
+  </si>
+  <si>
+    <t>Plantas de energia, tener otro proveedor de comunicaciones y control de copias de seguridad.Tener excelente locación de área de computo.</t>
+  </si>
+  <si>
+    <t>Hacer cambios en el plan de pruebas.</t>
+  </si>
+  <si>
+    <t>Actualizar la política de acuerdo a las normas de cada país</t>
+  </si>
+  <si>
+    <t>Hablar con el cliente. Generar un plan de cambio de políticas de tratamiento de datos. Hacer cambios pertinentes en el contrato respecto al tratamiento de datos.</t>
+  </si>
+  <si>
+    <t>No actualizar</t>
+  </si>
+  <si>
+    <t>Adquirir licencias a perpetuidad.O negociar contratos de licencia a largo plazo.Adquirir software con licencias libres.</t>
+  </si>
+  <si>
+    <t>Confirmar contrato sin cambio de condiciones.</t>
+  </si>
+  <si>
+    <t>Establecer condiciones en el contrato en caso de presentarse la situación.</t>
+  </si>
+  <si>
+    <t>Plantear un plan de negoción de negociación de costos.</t>
+  </si>
+  <si>
+    <t>Negociar costos.</t>
+  </si>
+  <si>
+    <t>Falta de cumplimiento de hitos por alguna area asociada al proyecto</t>
+  </si>
+  <si>
+    <t>Establecer fechas de entrega de cada uno de los hitos.</t>
+  </si>
+  <si>
+    <t>Hacer uso de la holgura establecida para entregas.Revisar Cronograma.</t>
+  </si>
+  <si>
+    <t>Establecer precio de producto basado en costos en moneda local considerando un margen de estabilidad y cobrar en moneda local del cliente.</t>
+  </si>
+  <si>
+    <t>Aplicar al cliente el costo de la tasa vigente</t>
+  </si>
+  <si>
+    <t>Asegurar los equipos, Generar un contrato de responsabilidad de uso.Elegir correcta locación.</t>
+  </si>
+  <si>
+    <t>Hacer reparaciones pertinenetes. Ir a la aseguradora. Cobrar daño al empleado.</t>
+  </si>
+  <si>
+    <t>Asegurar locación.Crear fondo de capital riesgo.</t>
+  </si>
+  <si>
+    <t>Acudir a la aseguradora. Invertir capital de riesgo.</t>
+  </si>
+  <si>
+    <t>Hacer buen levantamiento de requerimientos y delimitación de alcance</t>
+  </si>
+  <si>
+    <t>Mirar contrato.Renegociar contrato.</t>
+  </si>
+  <si>
+    <t>Ealuación de riesgos e impacto en las fases de desarrollo</t>
+  </si>
+  <si>
+    <t>Acceder a las previsoras de riesgo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -451,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -481,6 +622,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +652,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B31:C44" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B31:C44" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" name="Columna1"/>
-    <tableColumn id="2" name="Columna2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Columna1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Columna2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -765,11 +918,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:F55"/>
+    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1437,4 +1590,416 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C08A32-9E55-4306-A7F0-B282C12380AD}">
+  <dimension ref="B2:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="45">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="2:7" ht="78" customHeight="1">
+      <c r="B3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" ht="63.75" customHeight="1">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="2:7" s="16" customFormat="1" ht="102" customHeight="1">
+      <c r="B5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="2:7" ht="60">
+      <c r="B6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="2:7" ht="60">
+      <c r="B7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" ht="45">
+      <c r="B8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="2:7" ht="90">
+      <c r="B9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="2:7" ht="90">
+      <c r="B10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="2:7" ht="105">
+      <c r="B11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" ht="45">
+      <c r="B12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="2:7" ht="52.5" customHeight="1">
+      <c r="B13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="2:7" ht="90">
+      <c r="B14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" ht="45">
+      <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="2:7" ht="45">
+      <c r="B16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="2:7" ht="45">
+      <c r="B17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="2:7" ht="90">
+      <c r="B18" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="2:7" ht="75">
+      <c r="B19" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="2:7" ht="30">
+      <c r="B20" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="2:7" ht="60">
+      <c r="B21" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="2:7" ht="45">
+      <c r="B22" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="G26" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>